<commit_message>
1 record added in excel file
</commit_message>
<xml_diff>
--- a/Account Information.xlsx
+++ b/Account Information.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\UiPath\Queues_Dispatcher\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5237B9E2-2FCB-479B-AFDC-BE1622D841B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A31734A9-8A34-4A92-8033-017CD98AD7FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>First Name</t>
   </si>
@@ -121,6 +121,21 @@
   </si>
   <si>
     <t>anna.briggs@example.com</t>
+  </si>
+  <si>
+    <t>Partha</t>
+  </si>
+  <si>
+    <t>Saradhi</t>
+  </si>
+  <si>
+    <t>Pune, Maharashtra, 412207</t>
+  </si>
+  <si>
+    <t>886-766-2916</t>
+  </si>
+  <si>
+    <t>paardhu@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -185,10 +200,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -624,7 +640,27 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E7" s="1"/>
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7">
+        <v>43</v>
+      </c>
+      <c r="G7">
+        <v>4</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E8" s="1"/>

</xml_diff>